<commit_message>
Update modifications before ending municipality-level abm
</commit_message>
<xml_diff>
--- a/municipalities_abm/data/sbp_payments.xlsx
+++ b/municipalities_abm/data/sbp_payments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-abm\municipalities_abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F486ABC-6149-4271-9E27-F77F85D71D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006AA2CC-3EE6-4C9D-8B4C-EEF8E0367CEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="E7:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -370,34 +370,186 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>2009</v>
+        <v>1996</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2010</v>
+        <v>1997</v>
       </c>
       <c r="B3">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2011</v>
+        <v>1998</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>1999</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2000</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2001</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2002</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2003</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2004</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2005</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2006</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2007</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2008</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2009</v>
+      </c>
+      <c r="B15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2010</v>
+      </c>
+      <c r="B16">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2011</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>2012</v>
       </c>
-      <c r="B5">
+      <c r="B18">
         <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2013</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2014</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2015</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2016</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2017</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2018</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Munic-ABM: load soil, climate and census data
</commit_message>
<xml_diff>
--- a/municipalities_abm/data/sbp_payments.xlsx
+++ b/municipalities_abm/data/sbp_payments.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-abm\municipalities_abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006AA2CC-3EE6-4C9D-8B4C-EEF8E0367CEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80768E54-4C4E-482B-A0DF-F85FDD6F8058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,7 +39,7 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Payment</t>
+    <t>sbp_payment</t>
   </si>
 </sst>
 </file>
@@ -46,12 +55,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,7 +367,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="E7:G20"/>
+      <selection activeCell="B19" sqref="B19:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,7 +493,8 @@
         <v>2009</v>
       </c>
       <c r="B15">
-        <v>200</v>
+        <f>50.72+50.72+51.82</f>
+        <v>153.26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -485,15 +502,17 @@
         <v>2010</v>
       </c>
       <c r="B16">
-        <v>150</v>
+        <f>65.86+66.24</f>
+        <v>132.1</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2011</v>
       </c>
-      <c r="B17">
-        <v>100</v>
+      <c r="B17" s="1">
+        <f>40+43.58+43.45</f>
+        <v>127.03</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -501,7 +520,8 @@
         <v>2012</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <f>69.18+68.78</f>
+        <v>137.96</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -509,7 +529,7 @@
         <v>2013</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -517,7 +537,7 @@
         <v>2014</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Completeded municipalities ABM with ML insertion
</commit_message>
<xml_diff>
--- a/municipalities_abm/data/sbp_payments.xlsx
+++ b/municipalities_abm/data/sbp_payments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-abm\municipalities_abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80768E54-4C4E-482B-A0DF-F85FDD6F8058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753D3EE3-0BDA-48CC-ADA6-1D51783214E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
FL Toy ABM - Cash flows as input and corrected values
</commit_message>
<xml_diff>
--- a/municipalities_abm/data/sbp_payments.xlsx
+++ b/municipalities_abm/data/sbp_payments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\sbp-abm\municipalities_abm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753D3EE3-0BDA-48CC-ADA6-1D51783214E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB09D4CE-A7FC-414E-AF71-CA5EFDB492F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,8 +366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>